<commit_message>
Site updated: 2020-07-07 22:39:15
</commit_message>
<xml_diff>
--- a/data/flashcards.xlsx
+++ b/data/flashcards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mambawang\themes\next\source\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8705F2C3-69D3-4DC4-88AB-5FFD354D3A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25744BE4-BDCF-4511-8B40-67423087D4EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="124">
   <si>
     <t>Description</t>
   </si>
@@ -102,19 +102,10 @@
     <t>what is jvm</t>
   </si>
   <si>
-    <t>java virtual machine ,java程序需要在虚拟机上运行，所以可以跨平台</t>
-  </si>
-  <si>
     <t>what is jre</t>
   </si>
   <si>
-    <t>java runtime environment, 包括了jvm和java核心类库，主要是java.lang包</t>
-  </si>
-  <si>
     <t>what is jdk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">java development kit, java开发人员工具(比如javac.exe jar.exe等)，包含了jre, JDK &gt; JRE &gt; JVM </t>
   </si>
   <si>
     <t>JAVA</t>
@@ -266,15 +257,9 @@
     <t>还要考虑hashcode，因为A equal B，那么A的hashcode一定和B相同，但反过来就不一定</t>
   </si>
   <si>
-    <t>都可以作为逻辑与运算符，&amp;&amp;有短路功能，第一个false则不计算第二个参数，&amp;还可以做位运算符，按位与。</t>
-  </si>
-  <si>
     <t>static关键字</t>
   </si>
   <si>
-    <t>不需要创建实例对象就可以调用函数或者变量，只会在类加载的时候初始化一次。static里面只能调用static（因为没有对象），static方法可以直接通过类名调用</t>
-  </si>
-  <si>
     <t>先运行javac.exe 再运行java.exe</t>
   </si>
   <si>
@@ -299,30 +284,18 @@
     <t>int 和 Integer有什么区别</t>
   </si>
   <si>
-    <t>int是基本数据类型，Integer是包装类，int缺省是0，integer是null, integer需要实例化才能使用，int不需要</t>
-  </si>
-  <si>
     <t>线程安全</t>
   </si>
   <si>
-    <t>在一个线程访问时会加锁，同时只允许一个线程访问</t>
-  </si>
-  <si>
     <t>前者线程不安全，后者线程安全，当在多个线程中会访问到同一个对象的时候，才需要用到线程安全</t>
   </si>
   <si>
     <t>arraylist vector linkedlist</t>
   </si>
   <si>
-    <t>arraylist vector 采用的是数组的结构，查找快，插入慢，vector是线程安全的，相对来说性能就会差一点；linkedlist是双向链表，插入块，查找慢，需要遍历</t>
-  </si>
-  <si>
     <t>final finally finalize的区别</t>
   </si>
   <si>
-    <t>final关键字用来定义类方法和对象，分别作用是不可继承，不可覆盖，变量引用不可变；finally是异常检测代码的最后一部分，一定会执行；finalize是object类的一个方法，用于资源回收</t>
-  </si>
-  <si>
     <t>overload 和 override的区别</t>
   </si>
   <si>
@@ -362,39 +335,21 @@
     <t>float f = 3.4是否正确</t>
   </si>
   <si>
-    <t>错误，3.4是double型，属于向下转型（窄化）,需要强制转换，float f = (float)3.4 或者 float f = 3.4F</t>
-  </si>
-  <si>
     <t>java编码方式</t>
   </si>
   <si>
-    <t>unicode</t>
-  </si>
-  <si>
     <t>java四种访问修饰符</t>
   </si>
   <si>
     <t>private 私有，在同一类中可见，不可修饰类；缺省， 在同一包中可见；protected保护，同一包中可见，不可修饰类；public，其他包也可见</t>
   </si>
   <si>
-    <t>面向对象和面向过程的区别</t>
-  </si>
-  <si>
-    <t>面向过程是一步一步分析，最终完成目的，性能比较高；面向对象是模块化解决问题，低耦合，有封装继承多态的特性，便于维护和扩展；其实面向对象的底层还是面向过程，只不过被模块化了。</t>
-  </si>
-  <si>
-    <t>1.修饰类的时候不能被继承2. 修饰方法在子类中不会被重写3. 修饰变量的时候不能被更改数值或指向新的变量（不能再被new）    final变量如果直接被赋值而不是通过链接会被当成常量处理，final是指引用不能变，引用变量的内容是可以改变的。</t>
-  </si>
-  <si>
     <t>java支持多继承么</t>
   </si>
   <si>
     <t>不支持，但是可以通过内部类实现这一效果</t>
   </si>
   <si>
-    <t>java只支持参数传递</t>
-  </si>
-  <si>
     <t>方法得到的是所有参数值的一个拷贝，所以不能改变参数原本的值，但是可以改变对象参数的状态（比如数组中的值）</t>
   </si>
   <si>
@@ -419,9 +374,6 @@
     <t>sql</t>
   </si>
   <si>
-    <t>超键就是含有任意可以独立标识这个表的属性的集合；候选键就是不含有多余属性的超键；主键就是所有符合条件的候选键中选择一个，作为主键；外键就是R1表中的非主键，R2表中的主键</t>
-  </si>
-  <si>
     <t>join(inner join), left join, right join, full join</t>
   </si>
   <si>
@@ -440,12 +392,6 @@
     <t>用hashset可以，但会改变顺序，用linkedhashset最好</t>
   </si>
   <si>
-    <t>什么是封装</t>
-  </si>
-  <si>
-    <t>就是把对象的属性和方法包装起来，作为一个独立的整体；只提供相应的接口来访问数据，尽量做到隐藏对象的内部细节</t>
-  </si>
-  <si>
     <t>进程和线程</t>
   </si>
   <si>
@@ -470,15 +416,9 @@
     <t>hashmap底层如何实现</t>
   </si>
   <si>
-    <t>hashmap主要有put操作和get操作，put操作也就是存入数据的时候，先根据KEY值找到相应的bucket然后遍历这个bucket中的链表（树），找到key值，覆盖value,如果找不到，就在这个bucket头部插入这个value; 获取value的get操作，通过key确定bucket再获取相应的value</t>
-  </si>
-  <si>
     <t>indexing</t>
   </si>
   <si>
-    <t>索引分为聚集索引（索引的顺序和行的物理顺序是相同的，所以一个索引定位了，那么连续索引值的记录也一定跟在它后面，查找快，修改记录速度慢，类似于目录）和非聚集索引，是用来快速访问数据的</t>
-  </si>
-  <si>
     <t>创建线程</t>
   </si>
   <si>
@@ -491,7 +431,79 @@
     <t>编译时异常-》程序本身是没错的，但是外在的环境条件不满足则会触发，比如打开了不存在的端口，需要catch才能编译；运行时异常-》程序本身存在例如空指针，数组越界，0除数这种错误，需要修改程序，才能运行。</t>
   </si>
   <si>
-    <t>接口是抽象的合集1.接口不能实例化2.接口没有构造器3.接口方法都是抽象方法4.接口不能包含成员变量，除了static和final5.多继承</t>
+    <t>java程序员最重要的素质</t>
+  </si>
+  <si>
+    <t>1.should have standard, normalized coding habits 2. should be a good teamworker 3. should keep learning new techs cause world is changing 4.should have a good understanding skills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">java virtual machine ,java程序需要在虚拟机上运行，所以可以跨平台, all of the java program are running on jvm, which allows java programming on different platforms </t>
+  </si>
+  <si>
+    <t>java runtime environment, 包括了jvm和java核心类库，主要是java.lang包; jre contains jvm and the java core class library, such as java.lang</t>
+  </si>
+  <si>
+    <t>java development kit, java开发人员工具(比如javac.exe jar.exe等)，包含了jre, JDK &gt; JRE &gt; JVM ; it contains jre,jvm and some java developer machine such as javac.exe</t>
+  </si>
+  <si>
+    <t>都可以作为逻辑与运算符，&amp;&amp;有短路功能，第一个false则不计算第二个参数，&amp;还可以做位运算符，按位与. They can both be used as logic and operation, the single one can also be bit and operator, and the double one has short circuit, which means if the first parameter is false, it will not compute the next one</t>
+  </si>
+  <si>
+    <t>不需要创建实例对象就可以调用函数或者变量，只会在类加载的时候初始化一次。static里面只能调用static（因为没有对象），static方法可以直接通过类名调用; we don’t need a instance to call the method or attribute, we can ues the class name to call, and they will be initialized at the first time that the class was loaded.</t>
+  </si>
+  <si>
+    <t>1.修饰类的时候不能被继承2. 修饰方法在子类中不会被重写3. 修饰变量的时候不能被更改数值或指向新的变量（不能再被new）    final变量如果直接被赋值而不是通过链接会被当成常量处理，final是指引用不能变，引用变量的内容是可以改变的。Final can decorate calss, function and attribute</t>
+  </si>
+  <si>
+    <t>int是基本数据类型，Integer是包装类，int缺省是0，integer是null, integer需要实例化才能使用，int不需要; int is a basic data type of java and Integer is packed data type.</t>
+  </si>
+  <si>
+    <t>在一个线程访问时会加锁，同时只允许一个线程访问; at the same time only one thread can change the shared data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arraylist vector 采用的是数组的结构，查找快，插入慢，vector是线程安全的，相对来说性能就会差一点；linkedlist是双向链表，插入块，查找慢，需要遍历;arraylist and vector use array data structure and linkedlist use double ended linked list structure, only the vector is thread safe and the search is faster in array than linkedlist, insert is slower in array than the linkedlist </t>
+  </si>
+  <si>
+    <t>final关键字用来定义类方法和对象，分别作用是不可继承，不可覆盖，变量引用不可变；finally是异常检测代码的最后一部分，一定会执行；finalize是object类的一个方法，用于资源回收; finalize is a method of object class, it can be used for garbage collection.</t>
+  </si>
+  <si>
+    <t>错误，3.4是double型(more accuracy)，属于向下转型（窄化）,需要强制转换，float f = (float)3.4 或者 float f = 3.4F</t>
+  </si>
+  <si>
+    <t>unicode, one character has one code</t>
+  </si>
+  <si>
+    <t>面向对象和面向过程的区别(process-oriented)</t>
+  </si>
+  <si>
+    <t>什么是封装(encapsulation)</t>
+  </si>
+  <si>
+    <t>面向过程是一步一步分析，最终完成目的，性能比较高；面向对象是模块化解决问题，低耦合，有封装继承多态的特性，便于维护和扩展；其实面向对象的底层还是面向过程，只不过被模块化了。Process-o treats the question step by step, it will have better performance, oo will split the request in many parts, and each parts deal with different questions, then integrate all these parts to solve the problem.it will be more easier to change or mantain</t>
+  </si>
+  <si>
+    <t>java只支持参数传递(parameter passing)</t>
+  </si>
+  <si>
+    <t>接口是抽象的合集1.接口不能实例化2.接口没有构造器3.接口方法都是抽象方法4.接口不能包含成员变量，除了static和final5.多继承; interface cant be instanciated, has no constructor, allow multiple inheriated, only have abstract functions, no attributes</t>
+  </si>
+  <si>
+    <t>超键就是含有任意可以独立标识这个表的属性的集合；候选键就是不含有多余属性的超键；主键就是所有符合条件的候选键中选择一个，作为主键；外键就是R1表中的非主键，R2表中的主键; super key is the set of attributes that can unqiue represent the table  , candidate key is the super key without unncessary attributes, primary is one of the candidate key; foreign key is the primary key of othe table and not primary key of this table</t>
+  </si>
+  <si>
+    <t>就是把对象的属性和方法包装起来，作为一个独立的整体；只提供相应的接口来访问数据，尽量做到隐藏对象的内部细节; means pack the attributes and methods as a whole thing, only offer some interface to access the data to hide the detail of its inside.</t>
+  </si>
+  <si>
+    <t>hashmap主要有put操作和get操作，put操作也就是存入数据的时候，先根据KEY值找到相应的bucket然后遍历这个bucket中的链表（树），找到key值，覆盖value,如果找不到，就在这个bucket头部插入这个value; 获取value的get操作，通过key确定bucket再获取相应的value; we use put to store key-value pair, we first find the bucket of the key, then traverse the bucket to find its location and change the value, if we cant find this key in the bucket we insert the value at the top of the bucket.</t>
+  </si>
+  <si>
+    <t>索引分为聚集索引clusterd index（索引的顺序和行的物理顺序是相同的，所以一个索引定位了，那么连续索引值的记录也一定跟在它后面，查找快，修改记录速度慢，类似于目录）和非聚集索引nonclusered index，是用来快速访问数据的</t>
+  </si>
+  <si>
+    <t>array/arraylist</t>
+  </si>
+  <si>
+    <t>arrylist is a set, its dynamic, if we don’t know the capacity of the array, we can use arraylist to create the array and expand it later, if we know the capacity, we should use array.</t>
   </si>
 </sst>
 </file>
@@ -831,15 +843,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="99.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="94" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="89.44140625" style="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
@@ -957,7 +969,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -971,502 +983,524 @@
         <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
-        <v>81</v>
+        <v>113</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>